<commit_message>
Added User switches and LED to the pcb schematic
</commit_message>
<xml_diff>
--- a/ModelRocketAvionicsPCB/TM4C Pin Diagram.xlsx
+++ b/ModelRocketAvionicsPCB/TM4C Pin Diagram.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{F3F1C34A-C8B9-4366-BF1C-24E424E9CECA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{61CAABDE-F8B5-491D-8CB1-BE16BB3A5455}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{F3F1C34A-C8B9-4366-BF1C-24E424E9CECA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{3DFCEFCE-5CFD-401D-84C3-3E9B781F8DBE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="139">
   <si>
     <t>Pin Number</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Internal Positive Power Supply</t>
   </si>
   <si>
-    <t>PF0/SW_USR2</t>
-  </si>
-  <si>
     <t>User Push Button 2 and MCU Wake</t>
   </si>
   <si>
@@ -431,6 +428,15 @@
   </si>
   <si>
     <t>Other Functions/Peripherals</t>
+  </si>
+  <si>
+    <t>User Push Button 1</t>
+  </si>
+  <si>
+    <t>PF0/SW2</t>
+  </si>
+  <si>
+    <t>PF4/SW1</t>
   </si>
 </sst>
 </file>
@@ -1046,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1068,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>2</v>
@@ -1085,7 +1091,7 @@
         <v>62</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>3</v>
@@ -1102,7 +1108,7 @@
         <v>2</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -1164,6 +1170,12 @@
       <c r="C7" t="s">
         <v>2</v>
       </c>
+      <c r="D7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1318,13 +1330,13 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
         <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1336,13 +1348,13 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
         <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1360,7 +1372,7 @@
         <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,7 +1390,7 @@
         <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1396,7 +1408,7 @@
         <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1414,7 +1426,7 @@
         <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1509,10 +1521,10 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
+        <v>137</v>
+      </c>
+      <c r="E30" t="s">
         <v>79</v>
-      </c>
-      <c r="E30" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1527,10 +1539,10 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,7 +1584,7 @@
         <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1584,13 +1596,13 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D35" t="s">
         <v>35</v>
       </c>
       <c r="E35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1608,7 +1620,7 @@
         <v>36</v>
       </c>
       <c r="E36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1623,10 +1635,10 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37" t="s">
         <v>85</v>
-      </c>
-      <c r="E37" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1644,7 +1656,7 @@
         <v>38</v>
       </c>
       <c r="E38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1659,10 +1671,10 @@
         <v>3</v>
       </c>
       <c r="D39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" t="s">
         <v>87</v>
-      </c>
-      <c r="E39" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1677,10 +1689,10 @@
         <v>3</v>
       </c>
       <c r="D40" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" t="s">
         <v>89</v>
-      </c>
-      <c r="E40" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1717,7 +1729,7 @@
         <v>41</v>
       </c>
       <c r="E42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1735,7 +1747,7 @@
         <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1769,10 +1781,10 @@
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1787,10 +1799,10 @@
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1805,10 +1817,10 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" t="s">
         <v>94</v>
-      </c>
-      <c r="E47" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1823,10 +1835,10 @@
         <v>3</v>
       </c>
       <c r="D48" t="s">
+        <v>95</v>
+      </c>
+      <c r="E48" t="s">
         <v>96</v>
-      </c>
-      <c r="E48" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1841,10 +1853,10 @@
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1859,10 +1871,10 @@
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1877,10 +1889,10 @@
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1895,10 +1907,10 @@
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1913,10 +1925,10 @@
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1931,10 +1943,10 @@
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2042,10 +2054,10 @@
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2060,10 +2072,10 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E62" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2078,13 +2090,13 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E63" t="s">
+        <v>127</v>
+      </c>
+      <c r="F63" t="s">
         <v>128</v>
-      </c>
-      <c r="F63" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2099,13 +2111,13 @@
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E64" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2120,13 +2132,13 @@
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2141,13 +2153,13 @@
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>